<commit_message>
Check school ID issues on parsing redcap data
</commit_message>
<xml_diff>
--- a/tests/data/dispatch_list.xlsx
+++ b/tests/data/dispatch_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/rred-reports/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/rred-reports/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3792868D-9FC9-F648-96EF-2EEB5986DEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95993E3C-5CB7-744D-A2D4-03610092C464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2FAE3519-5632-8942-A48C-0ACAE4E3FF13}"/>
+    <workbookView xWindow="48000" yWindow="-960" windowWidth="19200" windowHeight="21100" xr2:uid="{2FAE3519-5632-8942-A48C-0ACAE4E3FF13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>School Label</t>
   </si>
@@ -120,13 +120,28 @@
   </si>
   <si>
     <t>leader_2@null.com</t>
+  </si>
+  <si>
+    <t>AB9234</t>
+  </si>
+  <si>
+    <t>AB100</t>
+  </si>
+  <si>
+    <t>AB101</t>
+  </si>
+  <si>
+    <t>another_school_180</t>
+  </si>
+  <si>
+    <t>UserID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,6 +161,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,10 +195,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -491,160 +515,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E54186F-C9D2-954F-9C31-FE1863ECE829}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="F4" t="s">
+      <c r="E4" s="2"/>
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{774E6E3B-A58C-A34D-81D6-F5102D83ECC6}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{A26F4DF7-CDA1-BB4B-9A86-9AC32248A863}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{F604E0A4-5948-9949-B8E7-7EC3F26CA5FD}"/>
-    <hyperlink ref="H2" r:id="rId4" xr:uid="{A6F306CB-72B3-9648-A70B-875F3F7A438C}"/>
-    <hyperlink ref="H3" r:id="rId5" xr:uid="{EBBFA0F2-5C80-F746-92C3-06DFAC2788E8}"/>
-    <hyperlink ref="H4" r:id="rId6" xr:uid="{C2EC7978-0A1E-9E49-B616-87838491BD15}"/>
-    <hyperlink ref="H5" r:id="rId7" xr:uid="{24F0A592-F768-B44C-BA63-FFA3F9FFA8C8}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{774E6E3B-A58C-A34D-81D6-F5102D83ECC6}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{A26F4DF7-CDA1-BB4B-9A86-9AC32248A863}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{F604E0A4-5948-9949-B8E7-7EC3F26CA5FD}"/>
+    <hyperlink ref="I2" r:id="rId4" xr:uid="{A6F306CB-72B3-9648-A70B-875F3F7A438C}"/>
+    <hyperlink ref="I3" r:id="rId5" xr:uid="{EBBFA0F2-5C80-F746-92C3-06DFAC2788E8}"/>
+    <hyperlink ref="I4" r:id="rId6" xr:uid="{C2EC7978-0A1E-9E49-B616-87838491BD15}"/>
+    <hyperlink ref="I5" r:id="rId7" xr:uid="{24F0A592-F768-B44C-BA63-FFA3F9FFA8C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>